<commit_message>
updated grades before final
</commit_message>
<xml_diff>
--- a/COSCGrades.xlsx
+++ b/COSCGrades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxcoplan/Documents/workspace/git/COSC336/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB87086-C0BB-1D4C-A006-56B1ECBDFFF4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF72D0D3-D5E1-9F4E-8051-85AECECC7720}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3920" yWindow="600" windowWidth="28040" windowHeight="17440" xr2:uid="{D5139097-3DF9-704E-976D-211727DE44E2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">a1 </t>
   </si>
@@ -87,12 +87,15 @@
   <si>
     <t>a8</t>
   </si>
+  <si>
+    <t>a9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -108,6 +111,21 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -133,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -142,11 +160,134 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -458,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9221883-BB25-4D46-8E4B-659E12299093}">
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q69" sqref="Q69"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -502,6 +643,9 @@
       </c>
       <c r="N1" s="3" t="s">
         <v>17</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -555,7 +699,7 @@
         <v>70</v>
       </c>
       <c r="Q3" s="5">
-        <f t="shared" ref="Q3:Q16" si="0">(0.35*AVERAGE(C3,E3:H3,J3:N3)+0.3*I3)/0.65</f>
+        <f t="shared" ref="Q3:Q15" si="0">(0.35*AVERAGE(C3,E3:H3,J3:N3)+0.3*I3)/0.65</f>
         <v>79.576923076923066</v>
       </c>
     </row>
@@ -937,9 +1081,12 @@
       <c r="N17" s="3">
         <v>90</v>
       </c>
+      <c r="O17" s="3">
+        <v>70</v>
+      </c>
       <c r="Q17">
-        <f>(0.35*AVERAGE(C17,E17:H17,J17:N17)+0.3*I17)/0.65</f>
-        <v>91.92307692307692</v>
+        <f>(0.35*AVERAGE(C17,E17:H17,J17:O17)+0.3*I17)/0.65</f>
+        <v>91.188811188811187</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -968,7 +1115,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
+      <c r="K19" s="8"/>
       <c r="L19" s="4"/>
       <c r="Q19" s="4"/>
     </row>
@@ -1308,9 +1455,18 @@
       <c r="L33" s="3">
         <v>90</v>
       </c>
+      <c r="M33" s="3">
+        <v>45</v>
+      </c>
+      <c r="N33" s="3">
+        <v>90</v>
+      </c>
+      <c r="O33" s="3">
+        <v>70</v>
+      </c>
       <c r="Q33">
-        <f>(0.35*AVERAGE(C33,E33:H33,J33:L33)+0.3*I33)/0.65</f>
-        <v>92.692307692307693</v>
+        <f>(0.35*AVERAGE(C33,E33:H33,J33:O33)+0.3*I33)/0.65</f>
+        <v>88.776223776223773</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -1468,9 +1624,18 @@
       <c r="L39" s="3">
         <v>70</v>
       </c>
+      <c r="M39" s="9">
+        <v>45</v>
+      </c>
+      <c r="N39" s="9">
+        <v>90</v>
+      </c>
+      <c r="O39" s="9">
+        <v>70</v>
+      </c>
       <c r="Q39">
-        <f>(0.35*AVERAGE(C39,E39:H39,J39:L39)+0.3*I39)/0.65</f>
-        <v>95.961538461538453</v>
+        <f>(0.35*AVERAGE(C39,E39:H39,J39:O39)+0.3*I39)/0.65</f>
+        <v>92.412587412587399</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -2086,9 +2251,18 @@
       <c r="L63" s="3">
         <v>100</v>
       </c>
+      <c r="M63" s="9">
+        <v>45</v>
+      </c>
+      <c r="N63" s="9">
+        <v>90</v>
+      </c>
+      <c r="O63" s="9">
+        <v>70</v>
+      </c>
       <c r="Q63">
-        <f>(0.35*AVERAGE(C63,E63:H63,J63:L63)+0.3*I63)/0.65</f>
-        <v>82.778846153846132</v>
+        <f>(0.35*AVERAGE(C63,E63:H63,J63:O63)+0.3*I63)/0.65</f>
+        <v>80.055944055944053</v>
       </c>
     </row>
     <row r="64" spans="1:17">
@@ -2302,9 +2476,9 @@
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="O70" s="3" t="e">
+      <c r="O70" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>70</v>
       </c>
       <c r="P70" s="3" t="e">
         <f t="shared" si="1"/>
@@ -2312,7 +2486,7 @@
       </c>
       <c r="Q70" s="3">
         <f>AVERAGE(Q3:Q67)</f>
-        <v>77.765124198717913</v>
+        <v>77.423805361305341</v>
       </c>
     </row>
     <row r="71" spans="1:17">
@@ -2369,7 +2543,7 @@
       </c>
       <c r="O71" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="P71" s="5">
         <f t="shared" si="2"/>
@@ -2434,7 +2608,7 @@
       </c>
       <c r="O72" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="P72" s="5">
         <f t="shared" si="3"/>
@@ -2497,9 +2671,9 @@
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-      <c r="O73" s="5" t="e">
+      <c r="O73" s="5">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
+        <v>70</v>
       </c>
       <c r="P73" s="5" t="e">
         <f t="shared" si="4"/>
@@ -2507,7 +2681,7 @@
       </c>
       <c r="Q73">
         <f>MEDIAN(Q3:Q67)</f>
-        <v>81.84615384615384</v>
+        <v>81.230769230769226</v>
       </c>
     </row>
     <row r="74" spans="1:17">
@@ -2554,17 +2728,17 @@
         <f t="shared" si="5"/>
         <v>26.428422928005723</v>
       </c>
-      <c r="M74" s="5" t="e">
+      <c r="M74" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N74" s="5" t="e">
+        <v>0</v>
+      </c>
+      <c r="N74" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O74" s="5" t="e">
+        <v>0</v>
+      </c>
+      <c r="O74" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P74" s="5" t="e">
         <f t="shared" si="5"/>
@@ -2572,13 +2746,29 @@
       </c>
       <c r="Q74">
         <f>STDEV(Q3:Q67)</f>
-        <v>14.710017126053712</v>
+        <v>14.419873331757021</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B69:B70"/>
   </mergeCells>
+  <conditionalFormatting sqref="C2:Q74">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q1:Q1048576">
+    <cfRule type="top10" dxfId="2" priority="2" percent="1" rank="16"/>
+    <cfRule type="top10" dxfId="1" priority="1" percent="1" bottom="1" rank="16"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final commit.  Nice working with you guys!
</commit_message>
<xml_diff>
--- a/COSCGrades.xlsx
+++ b/COSCGrades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxcoplan/Documents/workspace/git/COSC336/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662DD9DE-97ED-9D4B-B719-BE1593ACFDE2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D9FF55-8086-BC4A-9B0B-0EFA038D4115}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3920" yWindow="600" windowWidth="28040" windowHeight="17440" xr2:uid="{D5139097-3DF9-704E-976D-211727DE44E2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">a1 </t>
   </si>
@@ -64,9 +64,6 @@
     <t xml:space="preserve">q2 </t>
   </si>
   <si>
-    <t>Overall</t>
-  </si>
-  <si>
     <t>Average</t>
   </si>
   <si>
@@ -89,6 +86,15 @@
   </si>
   <si>
     <t>a9</t>
+  </si>
+  <si>
+    <t>Overall with final</t>
+  </si>
+  <si>
+    <t>Overall without final</t>
+  </si>
+  <si>
+    <t>Final</t>
   </si>
 </sst>
 </file>
@@ -151,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -162,11 +168,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="48">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -199,11 +216,421 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -537,15 +964,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9221883-BB25-4D46-8E4B-659E12299093}">
-  <dimension ref="A1:Q74"/>
+  <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="161" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="R68" sqref="R68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="17" max="17" width="23.6640625" customWidth="1"/>
+    <col min="18" max="18" width="20.5" style="9" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="6"/>
       <c r="B1" s="1"/>
       <c r="C1" s="6" t="s">
@@ -579,16 +1010,19 @@
         <v>9</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="P1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="6"/>
       <c r="B2" s="2"/>
       <c r="C2" s="6"/>
@@ -602,10 +1036,13 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="Q2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+        <v>19</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="4">
         <v>636</v>
       </c>
@@ -639,11 +1076,15 @@
         <v>70</v>
       </c>
       <c r="Q3" s="5">
-        <f t="shared" ref="Q3:Q15" si="0">(0.35*AVERAGE(C3,E3:H3,J3:N3)+0.3*I3)/0.65</f>
+        <f>(0.35*AVERAGE(C3,E3:H3,J3:N3)+0.3*I3)/0.65</f>
         <v>79.576923076923066</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" s="9">
+        <f t="shared" ref="R3:R16" si="0">(0.35*AVERAGE(C3,E3:H3,J3:O3)+0.3*I3+0.35*P3)/0.65</f>
+        <v>79.576923076923066</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -658,7 +1099,7 @@
       <c r="L4" s="3"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:18">
       <c r="A5" s="4">
         <v>972</v>
       </c>
@@ -688,11 +1129,15 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="Q5" s="5">
+        <f>(0.35*AVERAGE(C5,E5:H5,J5:N5)+0.3*I5)/0.65</f>
+        <v>57.230769230769219</v>
+      </c>
+      <c r="R5" s="9">
         <f t="shared" si="0"/>
         <v>57.230769230769219</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:18">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -707,7 +1152,7 @@
       <c r="L6" s="3"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:18">
       <c r="A7" s="4">
         <v>201</v>
       </c>
@@ -741,11 +1186,15 @@
         <v>40</v>
       </c>
       <c r="Q7" s="5">
+        <f>(0.35*AVERAGE(C7,E7:H7,J7:N7)+0.3*I7)/0.65</f>
+        <v>63.66346153846154</v>
+      </c>
+      <c r="R7" s="9">
         <f t="shared" si="0"/>
         <v>63.66346153846154</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:18">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -760,7 +1209,7 @@
       <c r="L8" s="3"/>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:18">
       <c r="A9" s="4">
         <v>432</v>
       </c>
@@ -796,11 +1245,15 @@
         <v>100</v>
       </c>
       <c r="Q9" s="5">
-        <f t="shared" si="0"/>
+        <f>(0.35*AVERAGE(C9,E9:H9,J9:N9)+0.3*I9)/0.65</f>
         <v>96.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="R9" s="9">
+        <f>(0.35*AVERAGE(C9,E9:H9,J9:O9)+0.3*I9+0.35*P9)</f>
+        <v>62.725000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -815,7 +1268,7 @@
       <c r="L10" s="3"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:18">
       <c r="A11" s="4">
         <v>931</v>
       </c>
@@ -851,11 +1304,15 @@
         <v>40</v>
       </c>
       <c r="Q11" s="5">
-        <f t="shared" si="0"/>
+        <f>(0.35*AVERAGE(C11,E11:H11,J11:N11)+0.3*I11)/0.65</f>
         <v>89.34615384615384</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="R11" s="9">
+        <f t="shared" ref="R10:R73" si="1">(0.35*AVERAGE(C11,E11:H11,J11:O11)+0.3*I11+0.35*P11)</f>
+        <v>58.074999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -870,7 +1327,7 @@
       <c r="L12" s="3"/>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:18">
       <c r="A13" s="4">
         <v>695</v>
       </c>
@@ -906,11 +1363,15 @@
         <v>70</v>
       </c>
       <c r="Q13" s="5">
-        <f t="shared" si="0"/>
+        <f>(0.35*AVERAGE(C13,E13:H13,J13:N13)+0.3*I13)/0.65</f>
         <v>63.038461538461526</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="R13" s="9">
+        <f t="shared" si="1"/>
+        <v>40.974999999999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -925,7 +1386,7 @@
       <c r="L14" s="3"/>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:18">
       <c r="A15" s="4">
         <v>237</v>
       </c>
@@ -961,11 +1422,15 @@
         <v>10</v>
       </c>
       <c r="Q15" s="5">
-        <f t="shared" si="0"/>
+        <f>(0.35*AVERAGE(C15,E15:H15,J15:N15)+0.3*I15)/0.65</f>
         <v>71.663461538461533</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="R15" s="9">
+        <f t="shared" si="1"/>
+        <v>46.581249999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -980,7 +1445,7 @@
       <c r="L16" s="3"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:18">
       <c r="A17" s="4">
         <v>756</v>
       </c>
@@ -1023,13 +1488,20 @@
       </c>
       <c r="O17" s="3">
         <v>70</v>
+      </c>
+      <c r="P17" s="3">
+        <v>90</v>
       </c>
       <c r="Q17">
         <f>(0.35*AVERAGE(C17,E17:H17,J17:O17)+0.3*I17)/0.65</f>
         <v>91.188811188811187</v>
       </c>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="R17" s="9">
+        <f>(0.35*AVERAGE(C17,E17:H17,J17:O17)+0.3*I17+0.35*P17)</f>
+        <v>90.772727272727266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1044,7 +1516,7 @@
       <c r="L18" s="4"/>
       <c r="Q18" s="4"/>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:18">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1059,7 +1531,7 @@
       <c r="L19" s="4"/>
       <c r="Q19" s="4"/>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:18">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1074,7 +1546,7 @@
       <c r="L20" s="4"/>
       <c r="Q20" s="4"/>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:18">
       <c r="A21" s="4">
         <v>0</v>
       </c>
@@ -1101,8 +1573,12 @@
         <f>(0.35*AVERAGE(C21,E21:H21,J21:L21)+0.3*I21)/0.65</f>
         <v>43.256410256410248</v>
       </c>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="R21" s="9">
+        <f t="shared" si="1"/>
+        <v>28.116666666666664</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1116,7 +1592,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:18">
       <c r="A23" s="4">
         <v>663</v>
       </c>
@@ -1153,8 +1629,12 @@
         <f>(0.35*AVERAGE(C23,E23:H23,J23:L23)+0.3*I23)/0.65</f>
         <v>85.894230769230759</v>
       </c>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="R23" s="9">
+        <f t="shared" si="1"/>
+        <v>55.831249999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1168,7 +1648,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:18">
       <c r="A25" s="4">
         <v>659</v>
       </c>
@@ -1205,8 +1685,12 @@
         <f>(0.35*AVERAGE(C25,E25:H25,J25:L25)+0.3*I25)/0.65</f>
         <v>85.807692307692307</v>
       </c>
-    </row>
-    <row r="26" spans="1:17">
+      <c r="R25" s="9">
+        <f t="shared" si="1"/>
+        <v>55.774999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1220,7 +1704,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:18">
       <c r="A27" s="4">
         <v>680</v>
       </c>
@@ -1255,8 +1739,12 @@
         <f>(0.35*AVERAGE(C27,E27:H27,J27:L27)+0.3*I27)/0.65</f>
         <v>73.179487179487168</v>
       </c>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="R27" s="9">
+        <f t="shared" si="1"/>
+        <v>47.566666666666663</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1270,7 +1758,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:18">
       <c r="A29" s="4">
         <v>400</v>
       </c>
@@ -1291,8 +1779,12 @@
         <f>(0.35*AVERAGE(C29,E29:H29,J29:L29)+0.3*I29)/0.65</f>
         <v>53.846153846153847</v>
       </c>
-    </row>
-    <row r="30" spans="1:17">
+      <c r="R29" s="9">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1306,7 +1798,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:18">
       <c r="A31" s="4">
         <v>486</v>
       </c>
@@ -1345,8 +1837,12 @@
         <f>(0.35*AVERAGE(C31,E31:H31,J31:L31)+0.3*I31)/0.65</f>
         <v>75.009615384615373</v>
       </c>
-    </row>
-    <row r="32" spans="1:17">
+      <c r="R31" s="9">
+        <f t="shared" si="1"/>
+        <v>48.756249999999994</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1360,7 +1856,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:18">
       <c r="A33" s="4">
         <v>340</v>
       </c>
@@ -1408,8 +1904,12 @@
         <f>(0.35*AVERAGE(C33,E33:H33,J33:O33)+0.3*I33)/0.65</f>
         <v>88.776223776223773</v>
       </c>
-    </row>
-    <row r="34" spans="1:17">
+      <c r="R33" s="9">
+        <f t="shared" si="1"/>
+        <v>57.704545454545453</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1423,7 +1923,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:18">
       <c r="A35" s="4">
         <v>245</v>
       </c>
@@ -1460,8 +1960,12 @@
         <f>(0.35*AVERAGE(C35,E35:H35,J35:L35)+0.3*I35)/0.65</f>
         <v>72.653846153846146</v>
       </c>
-    </row>
-    <row r="36" spans="1:17">
+      <c r="R35" s="9">
+        <f t="shared" si="1"/>
+        <v>47.224999999999994</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1475,7 +1979,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:18">
       <c r="A37" s="4">
         <v>628</v>
       </c>
@@ -1514,8 +2018,12 @@
         <f>(0.35*AVERAGE(C37,E37:H37,J37:L37)+0.3*I37)/0.65</f>
         <v>80.84615384615384</v>
       </c>
-    </row>
-    <row r="38" spans="1:17">
+      <c r="R37" s="9">
+        <f t="shared" si="1"/>
+        <v>52.55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1529,7 +2037,7 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:18">
       <c r="A39" s="4">
         <v>967</v>
       </c>
@@ -1572,13 +2080,20 @@
       </c>
       <c r="O39" s="8">
         <v>70</v>
+      </c>
+      <c r="P39" s="8">
+        <v>88</v>
       </c>
       <c r="Q39">
         <f>(0.35*AVERAGE(C39,E39:H39,J39:O39)+0.3*I39)/0.65</f>
         <v>92.412587412587399</v>
       </c>
-    </row>
-    <row r="40" spans="1:17">
+      <c r="R39" s="9">
+        <f t="shared" si="1"/>
+        <v>90.86818181818181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1592,7 +2107,7 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:18">
       <c r="A41" s="4">
         <v>663</v>
       </c>
@@ -1629,8 +2144,12 @@
         <f>(0.35*AVERAGE(C41,E41:H41,J41:L41)+0.3*I41)/0.65</f>
         <v>86.365384615384613</v>
       </c>
-    </row>
-    <row r="42" spans="1:17">
+      <c r="R41" s="9">
+        <f t="shared" si="1"/>
+        <v>56.137500000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1644,7 +2163,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:18">
       <c r="A43" s="4">
         <v>636</v>
       </c>
@@ -1681,8 +2200,12 @@
         <f>(0.35*AVERAGE(C43,E43:H43,J43:L43)+0.3*I43)/0.65</f>
         <v>83.163461538461533</v>
       </c>
-    </row>
-    <row r="44" spans="1:17">
+      <c r="R43" s="9">
+        <f t="shared" si="1"/>
+        <v>54.056249999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1696,7 +2219,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:18">
       <c r="A45" s="4">
         <v>847</v>
       </c>
@@ -1733,8 +2256,12 @@
         <f>(0.35*AVERAGE(C45,E45:H45,J45:L45)+0.3*I45)/0.65</f>
         <v>87.307692307692307</v>
       </c>
-    </row>
-    <row r="46" spans="1:17">
+      <c r="R45" s="9">
+        <f t="shared" si="1"/>
+        <v>56.75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1748,7 +2275,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:18">
       <c r="A47" s="4">
         <v>246</v>
       </c>
@@ -1787,8 +2314,12 @@
         <f>(0.35*AVERAGE(C47,E47:H47,J47:L47)+0.3*I47)/0.65</f>
         <v>74.961538461538453</v>
       </c>
-    </row>
-    <row r="48" spans="1:17">
+      <c r="R47" s="9">
+        <f t="shared" si="1"/>
+        <v>48.724999999999994</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1802,7 +2333,7 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:18">
       <c r="A49" s="4">
         <v>986</v>
       </c>
@@ -1839,8 +2370,12 @@
         <f>(0.35*AVERAGE(C49,E49:H49,J49:L49)+0.3*I49)/0.65</f>
         <v>81.615384615384613</v>
       </c>
-    </row>
-    <row r="50" spans="1:17">
+      <c r="R49" s="9">
+        <f t="shared" si="1"/>
+        <v>53.05</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -1854,7 +2389,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:18">
       <c r="A51" s="4">
         <v>550</v>
       </c>
@@ -1893,8 +2428,12 @@
         <f>(0.35*AVERAGE(C51,E51:H51,J51:L51)+0.3*I51)/0.65</f>
         <v>79.740384615384613</v>
       </c>
-    </row>
-    <row r="52" spans="1:17">
+      <c r="R51" s="9">
+        <f t="shared" si="1"/>
+        <v>51.831249999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -1908,7 +2447,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" spans="1:18">
       <c r="A53" s="4">
         <v>952</v>
       </c>
@@ -1947,8 +2486,12 @@
         <f>(0.35*AVERAGE(C53,E53:H53,J53:L53)+0.3*I53)/0.65</f>
         <v>96.038461538461533</v>
       </c>
-    </row>
-    <row r="54" spans="1:17">
+      <c r="R53" s="9">
+        <f t="shared" si="1"/>
+        <v>62.424999999999997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -1962,7 +2505,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="1:17">
+    <row r="55" spans="1:18">
       <c r="A55" s="4">
         <v>584</v>
       </c>
@@ -1999,8 +2542,12 @@
         <f>(0.35*AVERAGE(C55,E55:H55,J55:L55)+0.3*I55)/0.65</f>
         <v>82.153846153846146</v>
       </c>
-    </row>
-    <row r="56" spans="1:17">
+      <c r="R55" s="9">
+        <f t="shared" si="1"/>
+        <v>53.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -2014,7 +2561,7 @@
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="1:17">
+    <row r="57" spans="1:18">
       <c r="A57" s="4">
         <v>144</v>
       </c>
@@ -2045,8 +2592,12 @@
         <f>(0.35*AVERAGE(C57,E57:H57,J57:L57)+0.3*I57)/0.65</f>
         <v>57.723076923076917</v>
       </c>
-    </row>
-    <row r="58" spans="1:17">
+      <c r="R57" s="9">
+        <f t="shared" si="1"/>
+        <v>37.519999999999996</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="3"/>
@@ -2060,7 +2611,7 @@
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="1:17">
+    <row r="59" spans="1:18">
       <c r="A59" s="4">
         <v>747</v>
       </c>
@@ -2091,8 +2642,12 @@
         <f>(0.35*AVERAGE(C59,E59:H59,J59:L59)+0.3*I59)/0.65</f>
         <v>42.430769230769229</v>
       </c>
-    </row>
-    <row r="60" spans="1:17">
+      <c r="R59" s="9">
+        <f t="shared" si="1"/>
+        <v>27.58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -2106,7 +2661,7 @@
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="1:17">
+    <row r="61" spans="1:18">
       <c r="A61" s="4">
         <v>356</v>
       </c>
@@ -2141,8 +2696,12 @@
         <f>(0.35*AVERAGE(C61,E61:H61,J61:L61)+0.3*I61)/0.65</f>
         <v>82.076923076923066</v>
       </c>
-    </row>
-    <row r="62" spans="1:17">
+      <c r="R61" s="9">
+        <f t="shared" si="1"/>
+        <v>53.349999999999994</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -2156,7 +2715,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="1:17">
+    <row r="63" spans="1:18">
       <c r="A63" s="4">
         <v>733</v>
       </c>
@@ -2204,8 +2763,12 @@
         <f>(0.35*AVERAGE(C63,E63:H63,J63:O63)+0.3*I63)/0.65</f>
         <v>80.055944055944053</v>
       </c>
-    </row>
-    <row r="64" spans="1:17">
+      <c r="R63" s="9">
+        <f t="shared" si="1"/>
+        <v>52.036363636363632</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -2219,7 +2782,7 @@
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:17">
+    <row r="65" spans="1:18">
       <c r="A65" s="4">
         <v>279</v>
       </c>
@@ -2258,8 +2821,12 @@
         <f>(0.35*AVERAGE(C65,E65:H65,J65:L65)+0.3*I65)/0.65</f>
         <v>95.692307692307679</v>
       </c>
-    </row>
-    <row r="66" spans="1:17">
+      <c r="R65" s="9">
+        <f t="shared" si="1"/>
+        <v>62.199999999999996</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -2273,7 +2840,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:17">
+    <row r="67" spans="1:18">
       <c r="A67" s="4">
         <v>71</v>
       </c>
@@ -2310,8 +2877,12 @@
         <f>(0.35*AVERAGE(C67,E67:H67,J67:L67)+0.3*I67)/0.65</f>
         <v>84.346153846153854</v>
       </c>
-    </row>
-    <row r="68" spans="1:17">
+      <c r="R67" s="9">
+        <f t="shared" si="1"/>
+        <v>54.825000000000003</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -2325,11 +2896,11 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:17">
+    <row r="69" spans="1:18">
       <c r="A69" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B69" s="9"/>
+        <v>10</v>
+      </c>
+      <c r="B69" s="10"/>
       <c r="C69" s="3">
         <v>97</v>
       </c>
@@ -2364,329 +2935,353 @@
         <f>(0.35*AVERAGE(C69,E69:H69,J69:L69)+0.3*I69)/0.65</f>
         <v>81.021153846153837</v>
       </c>
-    </row>
-    <row r="70" spans="1:17">
+      <c r="R69" s="9">
+        <f t="shared" si="1"/>
+        <v>52.663749999999993</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18">
       <c r="A70" s="3"/>
-      <c r="B70" s="9"/>
+      <c r="B70" s="10"/>
       <c r="C70" s="3">
         <f>AVERAGE(C3:C67)</f>
         <v>97.290322580645167</v>
       </c>
       <c r="D70" s="3">
-        <f t="shared" ref="D70:P70" si="1">AVERAGE(D3:D67)</f>
+        <f t="shared" ref="D70:P70" si="2">AVERAGE(D3:D67)</f>
         <v>100</v>
       </c>
       <c r="E70" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70.535714285714292</v>
       </c>
       <c r="F70" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>84.645161290322577</v>
       </c>
       <c r="G70" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>83.862068965517238</v>
       </c>
       <c r="H70" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>86.896551724137936</v>
       </c>
       <c r="I70" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80.241379310344826</v>
       </c>
       <c r="J70" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>88.571428571428569</v>
       </c>
       <c r="K70" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>69.285714285714292</v>
       </c>
       <c r="L70" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>72.307692307692307</v>
       </c>
       <c r="M70" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="N70" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="O70" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="P70" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="P70" s="3">
+        <f t="shared" si="2"/>
+        <v>89</v>
       </c>
       <c r="Q70" s="3">
         <f>AVERAGE(Q3:Q67)</f>
         <v>77.423805361305341</v>
       </c>
-    </row>
-    <row r="71" spans="1:17">
+      <c r="R70" s="9">
+        <f t="shared" si="1"/>
+        <v>82.534970966186194</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18">
       <c r="A71" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C71">
         <f>MIN(C3:C67)</f>
         <v>50</v>
       </c>
       <c r="D71">
-        <f t="shared" ref="D71:P71" si="2">MIN(D3:D67)</f>
+        <f t="shared" ref="D71:P71" si="3">MIN(D3:D67)</f>
         <v>100</v>
       </c>
       <c r="E71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
       <c r="G71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="H71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="I71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="J71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>56</v>
       </c>
       <c r="K71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="L71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="M71" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="N71" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
       <c r="O71" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="P71" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>88</v>
       </c>
       <c r="Q71">
         <f>MIN(Q3:Q67)</f>
         <v>42.430769230769229</v>
       </c>
-    </row>
-    <row r="72" spans="1:17">
+      <c r="R71" s="9">
+        <f t="shared" si="1"/>
+        <v>57.15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C72">
         <f>MAX(C3:C67)</f>
         <v>100</v>
       </c>
       <c r="D72">
-        <f t="shared" ref="D72:P72" si="3">MAX(D3:D67)</f>
+        <f t="shared" ref="D72:P72" si="4">MAX(D3:D67)</f>
         <v>100</v>
       </c>
       <c r="E72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="F72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="G72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="H72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>94</v>
       </c>
       <c r="I72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>98</v>
       </c>
       <c r="K72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="L72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="M72" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="N72" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="O72" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="P72" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>90</v>
       </c>
       <c r="Q72">
         <f>MAX(Q3:Q67)</f>
         <v>96.5</v>
       </c>
-    </row>
-    <row r="73" spans="1:17">
+      <c r="R72" s="9">
+        <f t="shared" si="1"/>
+        <v>93.222727272727269</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C73">
         <f>MEDIAN(C3:C67)</f>
         <v>100</v>
       </c>
       <c r="D73">
-        <f t="shared" ref="D73:P73" si="4">MEDIAN(D3:D67)</f>
+        <f t="shared" ref="D73:P73" si="5">MEDIAN(D3:D67)</f>
         <v>100</v>
       </c>
       <c r="E73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
       <c r="F73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>84</v>
       </c>
       <c r="G73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>97</v>
       </c>
       <c r="H73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>90</v>
       </c>
       <c r="I73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>83</v>
       </c>
       <c r="J73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>89</v>
       </c>
       <c r="K73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>67.5</v>
       </c>
       <c r="L73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>70</v>
       </c>
       <c r="M73" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="N73" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>90</v>
       </c>
       <c r="O73" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>70</v>
       </c>
-      <c r="P73" s="5" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
+      <c r="P73" s="5">
+        <f t="shared" si="5"/>
+        <v>89</v>
       </c>
       <c r="Q73">
         <f>MEDIAN(Q3:Q67)</f>
         <v>81.230769230769226</v>
       </c>
-    </row>
-    <row r="74" spans="1:17">
+      <c r="R73" s="9">
+        <f t="shared" si="1"/>
+        <v>83.970454545454544</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18">
       <c r="A74" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C74">
         <f>STDEV(C3:C67)</f>
         <v>9.2671230644938021</v>
       </c>
       <c r="D74">
-        <f t="shared" ref="D74:P74" si="5">STDEV(D3:D67)</f>
+        <f t="shared" ref="D74:P74" si="6">STDEV(D3:D67)</f>
         <v>0</v>
       </c>
       <c r="E74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>33.370514977166145</v>
       </c>
       <c r="F74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11.768739346525248</v>
       </c>
       <c r="G74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>17.408380859170407</v>
       </c>
       <c r="H74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.9351322347378863</v>
       </c>
       <c r="I74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>16.302180337115729</v>
       </c>
       <c r="J74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.6280014903619655</v>
       </c>
       <c r="K74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>28.405603441544894</v>
       </c>
       <c r="L74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>26.428422928005723</v>
       </c>
       <c r="M74" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N74" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O74" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P74" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+      <c r="P74" s="5">
+        <f t="shared" si="6"/>
+        <v>1.4142135623730951</v>
       </c>
       <c r="Q74">
         <f>STDEV(Q3:Q67)</f>
         <v>14.419873331757021</v>
+      </c>
+      <c r="R74" s="9">
+        <f t="shared" ref="R74" si="7">(0.35*AVERAGE(C74,E74:H74,J74:O74)+0.3*I74+0.35*P74)</f>
+        <v>9.9423717043018609</v>
       </c>
     </row>
   </sheetData>
@@ -2694,7 +3289,7 @@
     <mergeCell ref="B69:B70"/>
   </mergeCells>
   <conditionalFormatting sqref="Q2:Q74">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2706,11 +3301,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="top10" dxfId="3" priority="3" percent="1" rank="16"/>
-    <cfRule type="top10" dxfId="2" priority="2" percent="1" bottom="1" rank="16"/>
+    <cfRule type="top10" dxfId="47" priority="9" percent="1" rank="16"/>
+    <cfRule type="top10" dxfId="46" priority="8" percent="1" bottom="1" rank="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:O73">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="C2:O73 P39 P17">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2721,6 +3316,22 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="R2:R74">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R1:R1048576">
+    <cfRule type="top10" dxfId="3" priority="1" percent="1" bottom="1" rank="16"/>
+    <cfRule type="top10" dxfId="2" priority="2" percent="1" rank="16"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>